<commit_message>
Almost done with linear regression
</commit_message>
<xml_diff>
--- a/training_schedule_updated.xlsx
+++ b/training_schedule_updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ron Tohar\Desktop\הכשרה\CV_training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A788F5A-A5EA-4BA1-8C41-22446266D96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F360F3-E109-4962-A155-F040D2F7292F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -454,7 +454,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -588,7 +588,7 @@
       </c>
       <c r="D12">
         <f>SUM(D13:D20)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -620,12 +620,18 @@
       <c r="C15">
         <v>1</v>
       </c>
+      <c r="D15">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>18</v>
       </c>
       <c r="C16">
+        <v>1.5</v>
+      </c>
+      <c r="D16">
         <v>1.5</v>
       </c>
     </row>

</xml_diff>